<commit_message>
done with export multiple xls
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -16,10 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name=" Gỗ Veener" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Chỉ tủ bếp dưới" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="Sheet1 (2)" r:id="rId8" sheetId="4"/>
-    <sheet name="Sheet1 (3)" r:id="rId9" sheetId="5"/>
-    <sheet name="Sheet1 (4)" r:id="rId10" sheetId="6"/>
-    <sheet name="Sheet1 (5)" r:id="rId11" sheetId="7"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -40,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="183">
   <si>
     <t>STT</t>
   </si>
@@ -639,10 +635,544 @@
   <si>
     <r>
       <rPr>
+        <b val="true"/>
         <sz val="12.0"/>
         <rFont val="Times New Roman"/>
       </rPr>
+      <t>I</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="14.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>NỘI THẤT PHÒNG KHÁCH</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="18.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>15,537,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Sofa tân cổ Italia</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Khung gỗ thông, bọc da hoặc nỉ công nghiệp Hàn Quốc, Giá trị tạm tính tính theo mẫu thực tế</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>0.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>800.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>750.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Mét dài</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>6,381,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
       <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Đôn ngồi sofa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>300.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>450.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Chiếc</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2,670,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>1.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Ghế ngồi sofa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>600.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Bộ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3,540,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">Bàn trà </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Giá trị ước tính ý nghĩa tham khảo, giá trị thực tính theo mẫu 3D hoặc lựa chọn mẫu thực tế</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>500.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>60.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>9,327,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Ốp tường</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Vách ốp nhựa in Bóng gương
+( In tranh, vân đá đối xứng, ...)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>5.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Mét vuông</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>1,398,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>6</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Kệ tivi</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">-Cánh: MDF chống ẩm  An Cường 25mm phủ sơn Inchem 5 lớp, soi họa tiết CNC
+-Thùng: MDF chống ẩm  An Cường 17mm  phủ sơn Inchem 5 lớp
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Hậu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">: MDF chống ẩm  An Cường 6mm  phủ sơn Inchem 5 lớp </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>400.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3,450,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>7</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Tủ trang trí (tủ rượu)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>350.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3,180,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Tủ giày Gỗ CN</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>3,440,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>9</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Đợt trang trí</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> MDF chống ẩm  An Cường phủ sơn Inchem 5 lớp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>34.0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>550,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>15,537,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>2,000,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>5,000,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>8,000,000</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12.0"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>537,000</t>
     </r>
   </si>
   <si>
@@ -663,7 +1193,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* \-??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="74">
+  <fonts count="263">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1021,6 +1551,780 @@
       <name val="Times New Roman"/>
       <sz val="13.0"/>
       <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="14.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="18.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <sz val="12.0"/>
     </font>
     <font>
       <name val="Times New Roman"/>
@@ -1265,7 +2569,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1686,6 +2990,285 @@
       <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="73" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="79" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="83" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="127" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="141" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="143" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="145" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="147" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="149" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="151" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="153" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="155" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="157" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="159" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="161" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="163" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="165" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="167" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="169" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="171" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="174" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="176" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="178" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="180" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="182" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="184" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="186" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="188" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="190" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="192" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="195" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="197" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="199" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="201" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="203" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="205" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="207" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="209" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="211" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="213" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="216" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="218" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="220" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="222" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="224" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="226" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="228" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="230" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="232" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="234" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="236" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="238" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="240" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="242" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="244" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="246" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="248" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="250" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="252" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="254" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="256" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="258" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="260" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="262" fillId="0" borderId="12" xfId="0" applyAlignment="true" applyBorder="true" applyFont="true">
       <alignment vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -2116,7 +3699,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -2350,131 +3933,435 @@
       <c r="J13" s="94"/>
       <c r="K13" s="89"/>
     </row>
-    <row r="14" spans="1:11" ht="47.85" customHeight="1">
-      <c r="A14" s="90" t="s">
+    <row r="14" ht="22.5" customHeight="true">
+      <c r="A14" t="s" s="136">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s" s="137">
+        <v>125</v>
+      </c>
+      <c r="C14" s="0"/>
+      <c r="D14" s="0"/>
+      <c r="E14" s="0"/>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" t="s" s="138">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="15" ht="40.0" customHeight="true">
+      <c r="A15" t="s" s="139">
+        <v>127</v>
+      </c>
+      <c r="B15" t="s" s="140">
+        <v>128</v>
+      </c>
+      <c r="C15" t="s" s="141">
+        <v>129</v>
+      </c>
+      <c r="D15" t="s" s="142">
+        <v>130</v>
+      </c>
+      <c r="E15" t="s" s="143">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s" s="144">
+        <v>132</v>
+      </c>
+      <c r="G15" t="s" s="145">
+        <v>133</v>
+      </c>
+      <c r="H15" t="s" s="146">
+        <v>134</v>
+      </c>
+      <c r="I15" t="s" s="147">
+        <v>130</v>
+      </c>
+      <c r="J15" t="s" s="148">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" ht="40.0" customHeight="true">
+      <c r="A16" t="s" s="149">
+        <v>136</v>
+      </c>
+      <c r="B16" t="s" s="150">
+        <v>137</v>
+      </c>
+      <c r="C16" t="s" s="151">
+        <v>129</v>
+      </c>
+      <c r="D16" t="s" s="152">
+        <v>138</v>
+      </c>
+      <c r="E16" t="s" s="153">
+        <v>138</v>
+      </c>
+      <c r="F16" t="s" s="154">
+        <v>139</v>
+      </c>
+      <c r="G16" t="s" s="155">
+        <v>140</v>
+      </c>
+      <c r="H16" t="s" s="156">
+        <v>141</v>
+      </c>
+      <c r="I16" t="s" s="157">
+        <v>142</v>
+      </c>
+      <c r="J16" t="s" s="158">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" ht="40.0" customHeight="true">
+      <c r="A17" t="s" s="159">
+        <v>143</v>
+      </c>
+      <c r="B17" t="s" s="160">
+        <v>144</v>
+      </c>
+      <c r="C17" t="s" s="161">
+        <v>129</v>
+      </c>
+      <c r="D17" t="s" s="162">
+        <v>131</v>
+      </c>
+      <c r="E17" t="s" s="163">
+        <v>145</v>
+      </c>
+      <c r="F17" t="s" s="164">
+        <v>139</v>
+      </c>
+      <c r="G17" t="s" s="165">
+        <v>146</v>
+      </c>
+      <c r="H17" t="s" s="166">
+        <v>147</v>
+      </c>
+      <c r="I17" t="s" s="167">
+        <v>142</v>
+      </c>
+      <c r="J17" t="s" s="168">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" ht="40.0" customHeight="true">
+      <c r="A18" t="s" s="169">
+        <v>148</v>
+      </c>
+      <c r="B18" t="s" s="170">
+        <v>149</v>
+      </c>
+      <c r="C18" t="s" s="171">
+        <v>150</v>
+      </c>
+      <c r="D18" t="s" s="172">
+        <v>151</v>
+      </c>
+      <c r="E18" t="s" s="173">
+        <v>152</v>
+      </c>
+      <c r="F18" t="s" s="174">
+        <v>151</v>
+      </c>
+      <c r="G18" t="s" s="175">
+        <v>140</v>
+      </c>
+      <c r="H18" t="s" s="176">
+        <v>153</v>
+      </c>
+      <c r="I18" t="s" s="177">
+        <v>142</v>
+      </c>
+      <c r="J18" t="s" s="178">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" ht="40.0" customHeight="true">
+      <c r="A19" t="s" s="179">
+        <v>154</v>
+      </c>
+      <c r="B19" t="s" s="180">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s" s="181">
+        <v>156</v>
+      </c>
+      <c r="D19" t="s" s="182">
+        <v>130</v>
+      </c>
+      <c r="E19" t="s" s="183">
+        <v>157</v>
+      </c>
+      <c r="F19" t="s" s="184">
+        <v>130</v>
+      </c>
+      <c r="G19" t="s" s="185">
+        <v>158</v>
+      </c>
+      <c r="H19" t="s" s="186">
+        <v>159</v>
+      </c>
+      <c r="I19" t="s" s="187">
+        <v>130</v>
+      </c>
+      <c r="J19" t="s" s="188">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" ht="77.5" customHeight="true">
+      <c r="A20" t="s" s="189">
+        <v>160</v>
+      </c>
+      <c r="B20" t="s" s="190">
+        <v>161</v>
+      </c>
+      <c r="C20" t="s" s="191">
+        <v>162</v>
+      </c>
+      <c r="D20" t="s" s="192">
+        <v>130</v>
+      </c>
+      <c r="E20" t="s" s="193">
+        <v>163</v>
+      </c>
+      <c r="F20" t="s" s="194">
+        <v>151</v>
+      </c>
+      <c r="G20" t="s" s="195">
+        <v>133</v>
+      </c>
+      <c r="H20" t="s" s="196">
+        <v>164</v>
+      </c>
+      <c r="I20" t="s" s="197">
+        <v>130</v>
+      </c>
+      <c r="J20" t="s" s="198">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" ht="77.5" customHeight="true">
+      <c r="A21" t="s" s="199">
+        <v>165</v>
+      </c>
+      <c r="B21" t="s" s="200">
+        <v>166</v>
+      </c>
+      <c r="C21" t="s" s="201">
+        <v>162</v>
+      </c>
+      <c r="D21" t="s" s="202">
+        <v>130</v>
+      </c>
+      <c r="E21" t="s" s="203">
+        <v>167</v>
+      </c>
+      <c r="F21" t="s" s="204">
+        <v>130</v>
+      </c>
+      <c r="G21" t="s" s="205">
+        <v>158</v>
+      </c>
+      <c r="H21" t="s" s="206">
+        <v>168</v>
+      </c>
+      <c r="I21" t="s" s="207">
+        <v>130</v>
+      </c>
+      <c r="J21" t="s" s="208">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" ht="77.5" customHeight="true">
+      <c r="A22" t="s" s="209">
+        <v>169</v>
+      </c>
+      <c r="B22" t="s" s="210">
+        <v>170</v>
+      </c>
+      <c r="C22" t="s" s="211">
+        <v>162</v>
+      </c>
+      <c r="D22" t="s" s="212">
+        <v>130</v>
+      </c>
+      <c r="E22" t="s" s="213">
+        <v>167</v>
+      </c>
+      <c r="F22" t="s" s="214">
+        <v>130</v>
+      </c>
+      <c r="G22" t="s" s="215">
+        <v>158</v>
+      </c>
+      <c r="H22" t="s" s="216">
+        <v>171</v>
+      </c>
+      <c r="I22" t="s" s="217">
+        <v>130</v>
+      </c>
+      <c r="J22" t="s" s="218">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" ht="40.0" customHeight="true">
+      <c r="A23" t="s" s="219">
+        <v>172</v>
+      </c>
+      <c r="B23" t="s" s="220">
+        <v>173</v>
+      </c>
+      <c r="C23" t="s" s="221">
+        <v>174</v>
+      </c>
+      <c r="D23" t="s" s="222">
+        <v>130</v>
+      </c>
+      <c r="E23" t="s" s="223">
+        <v>167</v>
+      </c>
+      <c r="F23" t="s" s="224">
+        <v>175</v>
+      </c>
+      <c r="G23" t="s" s="225">
+        <v>133</v>
+      </c>
+      <c r="H23" t="s" s="226">
+        <v>176</v>
+      </c>
+      <c r="I23" t="s" s="227">
+        <v>130</v>
+      </c>
+      <c r="J23" t="s" s="228">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="47.85" customHeight="1">
+      <c r="A24" s="90" t="s">
         <v>113</v>
       </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="11" t="s">
+      <c r="B24" s="90"/>
+      <c r="C24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="83" t="s">
+      <c r="D24" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="83" t="s">
+      <c r="E24" s="85"/>
+      <c r="F24" s="84"/>
+      <c r="G24" s="83" t="s">
         <v>112</v>
       </c>
-      <c r="H14" s="84"/>
-      <c r="I14" s="83" t="s">
+      <c r="H24" s="84"/>
+      <c r="I24" s="83" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="84"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="29.6" customHeight="true">
-      <c r="A15" s="136" t="s">
-        <v>124</v>
-      </c>
-      <c r="B15" s="91"/>
-      <c r="C15" s="137" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="138" t="s">
-        <v>124</v>
-      </c>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="139" t="s">
-        <v>124</v>
-      </c>
-      <c r="H15" s="88"/>
-      <c r="I15" s="140" t="s">
-        <v>124</v>
-      </c>
-      <c r="J15" s="88"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="93.45" customHeight="true">
-      <c r="A16" s="141" t="s">
-        <v>125</v>
-      </c>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A17" s="82" t="s">
+      <c r="J24" s="84"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" ht="29.6" customHeight="true">
+      <c r="A25" s="229" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" s="91"/>
+      <c r="C25" s="230" t="s">
+        <v>178</v>
+      </c>
+      <c r="D25" s="231" t="s">
+        <v>179</v>
+      </c>
+      <c r="E25" s="87"/>
+      <c r="F25" s="88"/>
+      <c r="G25" s="232" t="s">
+        <v>180</v>
+      </c>
+      <c r="H25" s="88"/>
+      <c r="I25" s="233" t="s">
+        <v>181</v>
+      </c>
+      <c r="J25" s="88"/>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:11" ht="93.45" customHeight="true">
+      <c r="A26" s="234" t="s">
+        <v>182</v>
+      </c>
+      <c r="B26" s="81"/>
+      <c r="C26" s="81"/>
+      <c r="D26" s="81"/>
+      <c r="E26" s="81"/>
+      <c r="F26" s="81"/>
+      <c r="G26" s="81"/>
+      <c r="H26" s="81"/>
+      <c r="I26" s="81"/>
+      <c r="J26" s="81"/>
+      <c r="K26" s="14"/>
+    </row>
+    <row r="27" spans="1:11" ht="16.149999999999999" customHeight="1">
+      <c r="A27" s="82" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="82" t="s">
+      <c r="B27" s="82"/>
+      <c r="C27" s="82"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="14"/>
+    </row>
+    <row r="28" spans="1:11" ht="16.149999999999999" customHeight="1">
+      <c r="A28" s="82"/>
+      <c r="B28" s="82"/>
+      <c r="C28" s="82"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" ht="17.45" customHeight="1">
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="K23" s="14"/>
-    </row>
-    <row r="32" spans="1:11" ht="17.45" customHeight="1"/>
-    <row r="33" ht="32.85" customHeight="1"/>
-    <row r="34" ht="16.149999999999999" customHeight="1"/>
-    <row r="35" ht="16.149999999999999" customHeight="1"/>
-    <row r="36" ht="16.149999999999999" customHeight="1"/>
-    <row r="37" ht="16.149999999999999" customHeight="1"/>
-    <row r="38" ht="16.149999999999999" customHeight="1"/>
-    <row r="39" ht="72.400000000000006" customHeight="1"/>
-    <row r="40" ht="13.9" customHeight="1"/>
-    <row r="41" ht="16.149999999999999" customHeight="1"/>
+      <c r="I28" s="82"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="14"/>
+    </row>
+    <row r="29" spans="1:11" ht="16.149999999999999" customHeight="1">
+      <c r="A29" s="82"/>
+      <c r="B29" s="82"/>
+      <c r="C29" s="82"/>
+      <c r="J29" s="16"/>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:11" ht="17.45" customHeight="1">
+      <c r="K30" s="14"/>
+    </row>
+    <row r="31" spans="1:11" ht="72.400000000000006" customHeight="1">
+      <c r="K31" s="14"/>
+    </row>
+    <row r="32" spans="1:11" ht="72.400000000000006" customHeight="1">
+      <c r="K32" s="14"/>
+    </row>
+    <row r="33" spans="1:11" ht="16.149999999999999" customHeight="1">
+      <c r="K33" s="14"/>
+    </row>
+    <row r="42" spans="1:11" ht="17.45" customHeight="1"/>
+    <row r="43" ht="32.85" customHeight="1"/>
+    <row r="44" ht="16.149999999999999" customHeight="1"/>
+    <row r="45" ht="16.149999999999999" customHeight="1"/>
+    <row r="46" ht="16.149999999999999" customHeight="1"/>
+    <row r="47" ht="16.149999999999999" customHeight="1"/>
+    <row r="48" ht="16.149999999999999" customHeight="1"/>
+    <row r="49" ht="72.400000000000006" customHeight="1"/>
+    <row r="50" ht="13.9" customHeight="1"/>
+    <row r="51" ht="16.149999999999999" customHeight="1"/>
   </sheetData>
-  <mergeCells count="32">
+  <mergeCells count="143">
     <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
     <mergeCell ref="A1:B5"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A12:A13"/>
@@ -2485,15 +4372,6 @@
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="J12:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A17:C19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
     <mergeCell ref="C1:J1"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C3:J3"/>
@@ -2504,6 +4382,18 @@
     <mergeCell ref="A9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:J11"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A27:C29"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="D24:F24"/>
+    <mergeCell ref="D25:F25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="I25:J25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -4242,1440 +6132,4 @@
     <oddFooter>&amp;RV1.0.08.2020</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K41"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="false" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="11.5703125"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125"/>
-    <col min="3" max="3" customWidth="true" width="50.140625"/>
-    <col min="4" max="6" customWidth="true" width="11.42578125"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.85546875"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="22.15" customHeight="1">
-      <c r="A6" s="93" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A12" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="95" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="89"/>
-    </row>
-    <row r="14" spans="1:11" ht="47.85" customHeight="1">
-      <c r="A14" s="90" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="83" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" s="84"/>
-      <c r="I14" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="84"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="90.95" customHeight="1">
-      <c r="A16" s="81"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A17" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" ht="17.45" customHeight="1">
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="K23" s="14"/>
-    </row>
-    <row r="32" spans="1:11" ht="17.45" customHeight="1"/>
-    <row r="33" ht="32.85" customHeight="1"/>
-    <row r="34" ht="16.149999999999999" customHeight="1"/>
-    <row r="35" ht="16.149999999999999" customHeight="1"/>
-    <row r="36" ht="16.149999999999999" customHeight="1"/>
-    <row r="37" ht="16.149999999999999" customHeight="1"/>
-    <row r="38" ht="16.149999999999999" customHeight="1"/>
-    <row r="39" ht="72.400000000000006" customHeight="1"/>
-    <row r="40" ht="13.9" customHeight="1"/>
-    <row r="41" ht="16.149999999999999" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A17:C19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0"/>
-  <headerFooter>
-    <oddFooter>&amp;RV1.0.08.2020</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K41"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="false" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="11.5703125"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125"/>
-    <col min="3" max="3" customWidth="true" width="50.140625"/>
-    <col min="4" max="6" customWidth="true" width="11.42578125"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.85546875"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="22.15" customHeight="1">
-      <c r="A6" s="93" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A12" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="95" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="89"/>
-    </row>
-    <row r="14" spans="1:11" ht="47.85" customHeight="1">
-      <c r="A14" s="90" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="83" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" s="84"/>
-      <c r="I14" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="84"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="90.95" customHeight="1">
-      <c r="A16" s="81"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A17" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" ht="17.45" customHeight="1">
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="K23" s="14"/>
-    </row>
-    <row r="32" spans="1:11" ht="17.45" customHeight="1"/>
-    <row r="33" ht="32.85" customHeight="1"/>
-    <row r="34" ht="16.149999999999999" customHeight="1"/>
-    <row r="35" ht="16.149999999999999" customHeight="1"/>
-    <row r="36" ht="16.149999999999999" customHeight="1"/>
-    <row r="37" ht="16.149999999999999" customHeight="1"/>
-    <row r="38" ht="16.149999999999999" customHeight="1"/>
-    <row r="39" ht="72.400000000000006" customHeight="1"/>
-    <row r="40" ht="13.9" customHeight="1"/>
-    <row r="41" ht="16.149999999999999" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A17:C19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0"/>
-  <headerFooter>
-    <oddFooter>&amp;RV1.0.08.2020</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K41"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="false" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="11.5703125"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125"/>
-    <col min="3" max="3" customWidth="true" width="50.140625"/>
-    <col min="4" max="6" customWidth="true" width="11.42578125"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.85546875"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="22.15" customHeight="1">
-      <c r="A6" s="93" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A12" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="95" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="89"/>
-    </row>
-    <row r="14" spans="1:11" ht="47.85" customHeight="1">
-      <c r="A14" s="90" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="83" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" s="84"/>
-      <c r="I14" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="84"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="90.95" customHeight="1">
-      <c r="A16" s="81"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A17" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" ht="17.45" customHeight="1">
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="K23" s="14"/>
-    </row>
-    <row r="32" spans="1:11" ht="17.45" customHeight="1"/>
-    <row r="33" ht="32.85" customHeight="1"/>
-    <row r="34" ht="16.149999999999999" customHeight="1"/>
-    <row r="35" ht="16.149999999999999" customHeight="1"/>
-    <row r="36" ht="16.149999999999999" customHeight="1"/>
-    <row r="37" ht="16.149999999999999" customHeight="1"/>
-    <row r="38" ht="16.149999999999999" customHeight="1"/>
-    <row r="39" ht="72.400000000000006" customHeight="1"/>
-    <row r="40" ht="13.9" customHeight="1"/>
-    <row r="41" ht="16.149999999999999" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A17:C19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0"/>
-  <headerFooter>
-    <oddFooter>&amp;RV1.0.08.2020</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:K41"/>
-  <sheetViews>
-    <sheetView showGridLines="0" tabSelected="false" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="11.5703125"/>
-    <col min="2" max="2" customWidth="true" width="24.42578125"/>
-    <col min="3" max="3" customWidth="true" width="50.140625"/>
-    <col min="4" max="6" customWidth="true" width="11.42578125"/>
-    <col min="7" max="7" customWidth="true" width="13.85546875"/>
-    <col min="8" max="8" customWidth="true" width="20.0"/>
-    <col min="9" max="9" customWidth="true" width="12.85546875"/>
-    <col min="10" max="10" customWidth="true" width="20.0"/>
-    <col min="11" max="11" customWidth="true" hidden="true" width="37.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="37.5" customHeight="1">
-      <c r="A1" s="92"/>
-      <c r="B1" s="92"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2"/>
-    </row>
-    <row r="2" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A2" s="92"/>
-      <c r="B2" s="92"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="3"/>
-    </row>
-    <row r="3" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A3" s="92"/>
-      <c r="B3" s="92"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A4" s="92"/>
-      <c r="B4" s="92"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="3"/>
-    </row>
-    <row r="5" spans="1:11" ht="29.1" customHeight="1">
-      <c r="A5" s="92"/>
-      <c r="B5" s="92"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" ht="22.15" customHeight="1">
-      <c r="A6" s="93" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="93"/>
-      <c r="D6" s="93"/>
-      <c r="E6" s="93"/>
-      <c r="F6" s="93"/>
-      <c r="G6" s="93"/>
-      <c r="H6" s="93"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="16.5">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="7"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-    </row>
-    <row r="10" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="7"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="7"/>
-    </row>
-    <row r="12" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A12" s="94" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="94" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="94" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" s="95"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="94" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="94" t="s">
-        <v>5</v>
-      </c>
-      <c r="I12" s="95" t="s">
-        <v>6</v>
-      </c>
-      <c r="J12" s="95" t="s">
-        <v>7</v>
-      </c>
-      <c r="K12" s="89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="94"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="94"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="89"/>
-    </row>
-    <row r="14" spans="1:11" ht="47.85" customHeight="1">
-      <c r="A14" s="90" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14" s="90"/>
-      <c r="C14" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="83" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="85"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="83" t="s">
-        <v>112</v>
-      </c>
-      <c r="H14" s="84"/>
-      <c r="I14" s="83" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="84"/>
-      <c r="K14" s="12"/>
-    </row>
-    <row r="15" spans="1:11" ht="17.100000000000001" customHeight="1">
-      <c r="A15" s="91"/>
-      <c r="B15" s="91"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="86"/>
-      <c r="E15" s="87"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="86"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="14"/>
-    </row>
-    <row r="16" spans="1:11" ht="90.95" customHeight="1">
-      <c r="A16" s="81"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="81"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="81"/>
-      <c r="G16" s="81"/>
-      <c r="H16" s="81"/>
-      <c r="I16" s="81"/>
-      <c r="J16" s="81"/>
-      <c r="K16" s="14"/>
-    </row>
-    <row r="17" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A17" s="82" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="82"/>
-      <c r="C17" s="82"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-    </row>
-    <row r="18" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A18" s="82"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="82" t="s">
-        <v>16</v>
-      </c>
-      <c r="I18" s="82"/>
-      <c r="J18" s="16"/>
-      <c r="K18" s="14"/>
-    </row>
-    <row r="19" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="A19" s="82"/>
-      <c r="B19" s="82"/>
-      <c r="C19" s="82"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="14"/>
-    </row>
-    <row r="20" spans="1:11" ht="17.45" customHeight="1">
-      <c r="K20" s="14"/>
-    </row>
-    <row r="21" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K21" s="14"/>
-    </row>
-    <row r="22" spans="1:11" ht="72.400000000000006" customHeight="1">
-      <c r="K22" s="14"/>
-    </row>
-    <row r="23" spans="1:11" ht="16.149999999999999" customHeight="1">
-      <c r="K23" s="14"/>
-    </row>
-    <row r="32" spans="1:11" ht="17.45" customHeight="1"/>
-    <row r="33" ht="32.85" customHeight="1"/>
-    <row r="34" ht="16.149999999999999" customHeight="1"/>
-    <row r="35" ht="16.149999999999999" customHeight="1"/>
-    <row r="36" ht="16.149999999999999" customHeight="1"/>
-    <row r="37" ht="16.149999999999999" customHeight="1"/>
-    <row r="38" ht="16.149999999999999" customHeight="1"/>
-    <row r="39" ht="72.400000000000006" customHeight="1"/>
-    <row r="40" ht="13.9" customHeight="1"/>
-    <row r="41" ht="16.149999999999999" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A1:B5"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="A16:J16"/>
-    <mergeCell ref="A17:C19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="D14:F14"/>
-    <mergeCell ref="D15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:J15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0"/>
-  <headerFooter>
-    <oddFooter>&amp;RV1.0.08.2020</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>